<commit_message>
Added the re-analyzed TCRBOA6 example with all used scripts and the correct target regions .bed file.
</commit_message>
<xml_diff>
--- a/Examples/somaticGermline_TCRBOA6/All_Mutations_Somatic_LoH.xlsx
+++ b/Examples/somaticGermline_TCRBOA6/All_Mutations_Somatic_LoH.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="233">
   <si>
     <t xml:space="preserve">Symbol</t>
   </si>
@@ -56,7 +56,7 @@
     <t xml:space="preserve">CLINSIG</t>
   </si>
   <si>
-    <t xml:space="preserve">COSMIC84</t>
+    <t xml:space="preserve">COSMIC86</t>
   </si>
   <si>
     <t xml:space="preserve">PLEKHM2</t>
@@ -80,6 +80,9 @@
     <t xml:space="preserve">.</t>
   </si>
   <si>
+    <t xml:space="preserve">34</t>
+  </si>
+  <si>
     <t xml:space="preserve">D</t>
   </si>
   <si>
@@ -107,6 +110,9 @@
     <t xml:space="preserve">p.Leu316*</t>
   </si>
   <si>
+    <t xml:space="preserve">35</t>
+  </si>
+  <si>
     <t xml:space="preserve">N</t>
   </si>
   <si>
@@ -125,6 +131,9 @@
     <t xml:space="preserve">p.Glu199Gly</t>
   </si>
   <si>
+    <t xml:space="preserve">23.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">NEUROD1</t>
   </si>
   <si>
@@ -140,6 +149,9 @@
     <t xml:space="preserve">p.Lys39Glu</t>
   </si>
   <si>
+    <t xml:space="preserve">10.67</t>
+  </si>
+  <si>
     <t xml:space="preserve">DOCK3</t>
   </si>
   <si>
@@ -155,6 +167,9 @@
     <t xml:space="preserve">p.Leu1633Phe</t>
   </si>
   <si>
+    <t xml:space="preserve">19.08</t>
+  </si>
+  <si>
     <t xml:space="preserve">GPR156</t>
   </si>
   <si>
@@ -170,21 +185,27 @@
     <t xml:space="preserve">p.Ala608Val</t>
   </si>
   <si>
+    <t xml:space="preserve">20.9</t>
+  </si>
+  <si>
     <t xml:space="preserve">UNC5C</t>
   </si>
   <si>
     <t xml:space="preserve">unc-5 netrin receptor C</t>
   </si>
   <si>
-    <t xml:space="preserve">38.82%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">59|152</t>
+    <t xml:space="preserve">39.22%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60|153</t>
   </si>
   <si>
     <t xml:space="preserve">p.Pro839Ser</t>
   </si>
   <si>
+    <t xml:space="preserve">23.8</t>
+  </si>
+  <si>
     <t xml:space="preserve">ID=COSM2989103;OCCURENCE=2(large_intestine)</t>
   </si>
   <si>
@@ -203,6 +224,9 @@
     <t xml:space="preserve">p.Ser613Phe</t>
   </si>
   <si>
+    <t xml:space="preserve">11.51</t>
+  </si>
+  <si>
     <t xml:space="preserve">MEGF10</t>
   </si>
   <si>
@@ -218,19 +242,7 @@
     <t xml:space="preserve">p.Ala726Val</t>
   </si>
   <si>
-    <t xml:space="preserve">LCP2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lymphocyte cytosolic protein 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34.41%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">96|283</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p.Ala143Val</t>
+    <t xml:space="preserve">24.8</t>
   </si>
   <si>
     <t xml:space="preserve">ATP6V0A4</t>
@@ -248,6 +260,9 @@
     <t xml:space="preserve">p.Ala706Ser</t>
   </si>
   <si>
+    <t xml:space="preserve">1.999</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANKRD30A</t>
   </si>
   <si>
@@ -263,6 +278,9 @@
     <t xml:space="preserve">p.Cys516Tyr</t>
   </si>
   <si>
+    <t xml:space="preserve">0.001</t>
+  </si>
+  <si>
     <t xml:space="preserve">28.12%</t>
   </si>
   <si>
@@ -272,22 +290,7 @@
     <t xml:space="preserve">p.Cys873Tyr</t>
   </si>
   <si>
-    <t xml:space="preserve">MUC2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mucin 2, oligomeric mucus/gel-forming</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16.33%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8|51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p.Ser1698Thr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID=COSM4184070,COSM4184071;OCCURENCE=1(bone),2(liver),1(thyroid),1(large_intestine)</t>
+    <t xml:space="preserve">6.906</t>
   </si>
   <si>
     <t xml:space="preserve">ZC3H10</t>
@@ -305,6 +308,9 @@
     <t xml:space="preserve">p.Val181Asp</t>
   </si>
   <si>
+    <t xml:space="preserve">9.774</t>
+  </si>
+  <si>
     <t xml:space="preserve">LCTL</t>
   </si>
   <si>
@@ -320,6 +326,27 @@
     <t xml:space="preserve">p.Thr36Ile</t>
   </si>
   <si>
+    <t xml:space="preserve">23.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD177 molecule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33.83%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68|202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.Val240Met</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.844</t>
+  </si>
+  <si>
     <t xml:space="preserve">TMC2</t>
   </si>
   <si>
@@ -338,6 +365,9 @@
     <t xml:space="preserve">p.Lys165*</t>
   </si>
   <si>
+    <t xml:space="preserve">37</t>
+  </si>
+  <si>
     <t xml:space="preserve">CYBB</t>
   </si>
   <si>
@@ -353,6 +383,9 @@
     <t xml:space="preserve">p.Gly512Arg</t>
   </si>
   <si>
+    <t xml:space="preserve">32</t>
+  </si>
+  <si>
     <t xml:space="preserve">VHL</t>
   </si>
   <si>
@@ -362,10 +395,10 @@
     <t xml:space="preserve">frameshift deletion</t>
   </si>
   <si>
-    <t xml:space="preserve">51.49%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">52|101</t>
+    <t xml:space="preserve">50.98%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">52|102</t>
   </si>
   <si>
     <t xml:space="preserve"> p.His125fs</t>
@@ -389,27 +422,6 @@
     <t xml:space="preserve">62|112</t>
   </si>
   <si>
-    <t xml:space="preserve">KRTAP9-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">keratin associated protein 9-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nonframeshift deletion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.51%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10|75</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> p.Thr152_Cys153delinsSer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID=COSM1134046,COSM436567;OCCURENCE=2(breast),2(skin),6(thyroid),1(upper_aerodigestive_tract)</t>
-  </si>
-  <si>
     <t xml:space="preserve">CEACAM8</t>
   </si>
   <si>
@@ -440,6 +452,9 @@
     <t xml:space="preserve">p.Ala77Val</t>
   </si>
   <si>
+    <t xml:space="preserve">3.410</t>
+  </si>
+  <si>
     <t xml:space="preserve">ARIH2OS</t>
   </si>
   <si>
@@ -455,6 +470,27 @@
     <t xml:space="preserve">p.Ser166Pro</t>
   </si>
   <si>
+    <t xml:space="preserve">13.20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FILIP1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filamin A interacting protein 1 like</t>
+  </si>
+  <si>
+    <t xml:space="preserve">85.45%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47|55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.Lys183Glu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.25</t>
+  </si>
+  <si>
     <t xml:space="preserve">NFKBIZ</t>
   </si>
   <si>
@@ -470,6 +506,9 @@
     <t xml:space="preserve">p.Leu545Pro</t>
   </si>
   <si>
+    <t xml:space="preserve">27.2</t>
+  </si>
+  <si>
     <t xml:space="preserve">LSG1</t>
   </si>
   <si>
@@ -485,19 +524,7 @@
     <t xml:space="preserve">p.Leu510Phe</t>
   </si>
   <si>
-    <t xml:space="preserve">ABTB2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ankyrin repeat and BTB domain containing 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">90.24%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37|41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p.Arg452Gln</t>
+    <t xml:space="preserve">23.3</t>
   </si>
   <si>
     <t xml:space="preserve">TNKS1BP1</t>
@@ -533,6 +560,9 @@
     <t xml:space="preserve">p.Gln694Arg</t>
   </si>
   <si>
+    <t xml:space="preserve">6.974</t>
+  </si>
+  <si>
     <t xml:space="preserve">LTBP3</t>
   </si>
   <si>
@@ -548,37 +578,19 @@
     <t xml:space="preserve">p.Pro488Ser</t>
   </si>
   <si>
-    <t xml:space="preserve">ACY3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aminoacylase 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">77.98%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">85|109</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p.Thr277Arg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MYO7A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">myosin VIIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79.59%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78|99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p.Val411Ala</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Uncertain significance</t>
+    <t xml:space="preserve">12.94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZNF705E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zinc finger protein 705E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76.8%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">96|125</t>
   </si>
   <si>
     <t xml:space="preserve">ALKBH8</t>
@@ -596,6 +608,9 @@
     <t xml:space="preserve">p.Ser149Cys</t>
   </si>
   <si>
+    <t xml:space="preserve">24.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANKK1</t>
   </si>
   <si>
@@ -611,19 +626,19 @@
     <t xml:space="preserve">p.Arg295Cys</t>
   </si>
   <si>
-    <t xml:space="preserve">NECTIN1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nectin cell adhesion molecule 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75.81%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">94|125</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p.Gly480Ser</t>
+    <t xml:space="preserve">14.80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISG20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interferon stimulated exonuclease gene 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.97%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50|61</t>
   </si>
   <si>
     <t xml:space="preserve">ZNF521</t>
@@ -641,6 +656,9 @@
     <t xml:space="preserve">p.Glu484Lys</t>
   </si>
   <si>
+    <t xml:space="preserve">21.9</t>
+  </si>
+  <si>
     <t xml:space="preserve">ID=COSM6830919;OCCURENCE=1(large_intestine)</t>
   </si>
   <si>
@@ -659,6 +677,9 @@
     <t xml:space="preserve">p.Ser95Arg</t>
   </si>
   <si>
+    <t xml:space="preserve">23.4</t>
+  </si>
+  <si>
     <t xml:space="preserve">BRWD1</t>
   </si>
   <si>
@@ -672,6 +693,24 @@
   </si>
   <si>
     <t xml:space="preserve">p.Thr1205Ile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9orf147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chromosome 9 open reading frame 147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16|16</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1086,37 +1125,37 @@
       <c r="K2" t="n">
         <v>0.000009314</v>
       </c>
-      <c r="L2" t="n">
-        <v>34</v>
+      <c r="L2" t="s">
+        <v>22</v>
       </c>
       <c r="M2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -1131,78 +1170,78 @@
         <v>21</v>
       </c>
       <c r="K3"/>
-      <c r="L3" t="n">
-        <v>35</v>
+      <c r="L3" t="s">
+        <v>32</v>
       </c>
       <c r="M3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4"/>
+      <c r="L4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" t="s">
         <v>33</v>
       </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4"/>
-      <c r="L4" t="n">
-        <v>23.1</v>
-      </c>
-      <c r="M4" t="s">
-        <v>31</v>
-      </c>
       <c r="N4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -1217,35 +1256,35 @@
         <v>21</v>
       </c>
       <c r="K5"/>
-      <c r="L5" t="n">
-        <v>10.67</v>
+      <c r="L5" t="s">
+        <v>45</v>
       </c>
       <c r="M5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -1262,35 +1301,35 @@
       <c r="K6" t="n">
         <v>0</v>
       </c>
-      <c r="L6" t="n">
-        <v>19.08</v>
+      <c r="L6" t="s">
+        <v>51</v>
       </c>
       <c r="M6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="F7" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -1305,35 +1344,35 @@
         <v>21</v>
       </c>
       <c r="K7"/>
-      <c r="L7" t="n">
-        <v>20.9</v>
+      <c r="L7" t="s">
+        <v>57</v>
       </c>
       <c r="M7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -1348,37 +1387,37 @@
         <v>21</v>
       </c>
       <c r="K8"/>
-      <c r="L8" t="n">
-        <v>23.8</v>
+      <c r="L8" t="s">
+        <v>63</v>
       </c>
       <c r="M8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O8" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="F9" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -1393,35 +1432,35 @@
         <v>21</v>
       </c>
       <c r="K9"/>
-      <c r="L9" t="n">
-        <v>11.51</v>
+      <c r="L9" t="s">
+        <v>70</v>
       </c>
       <c r="M9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -1436,35 +1475,35 @@
         <v>21</v>
       </c>
       <c r="K10"/>
-      <c r="L10" t="n">
-        <v>24.8</v>
+      <c r="L10" t="s">
+        <v>76</v>
       </c>
       <c r="M10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C11" t="s">
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="F11" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -1478,38 +1517,36 @@
       <c r="J11" t="s">
         <v>21</v>
       </c>
-      <c r="K11" t="n">
-        <v>0.0001</v>
-      </c>
-      <c r="L11" t="n">
-        <v>23</v>
+      <c r="K11"/>
+      <c r="L11" t="s">
+        <v>82</v>
       </c>
       <c r="M11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="F12" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -1524,35 +1561,35 @@
         <v>21</v>
       </c>
       <c r="K12"/>
-      <c r="L12" t="n">
-        <v>1.999</v>
+      <c r="L12" t="s">
+        <v>88</v>
       </c>
       <c r="M12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O12"/>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="E13" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="F13" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -1567,35 +1604,35 @@
         <v>21</v>
       </c>
       <c r="K13"/>
-      <c r="L13" t="n">
-        <v>0.001</v>
+      <c r="L13" t="s">
+        <v>92</v>
       </c>
       <c r="M13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O13"/>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="E14" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="F14" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
@@ -1610,35 +1647,35 @@
         <v>21</v>
       </c>
       <c r="K14"/>
-      <c r="L14" t="n">
-        <v>6.906</v>
+      <c r="L14" t="s">
+        <v>98</v>
       </c>
       <c r="M14" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C15" t="s">
         <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="E15" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="F15" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
@@ -1653,37 +1690,35 @@
         <v>21</v>
       </c>
       <c r="K15"/>
-      <c r="L15" t="n">
-        <v>0.646</v>
+      <c r="L15" t="s">
+        <v>104</v>
       </c>
       <c r="M15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N15" t="s">
-        <v>23</v>
-      </c>
-      <c r="O15" t="s">
-        <v>91</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="O15"/>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="B16" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="E16" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="F16" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
@@ -1698,35 +1733,33 @@
         <v>21</v>
       </c>
       <c r="K16"/>
-      <c r="L16" t="n">
-        <v>9.774</v>
-      </c>
-      <c r="M16" t="s">
-        <v>31</v>
-      </c>
+      <c r="L16" t="s">
+        <v>110</v>
+      </c>
+      <c r="M16"/>
       <c r="N16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O16"/>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="B17" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="D17" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="E17" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="F17" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
@@ -1741,35 +1774,33 @@
         <v>21</v>
       </c>
       <c r="K17"/>
-      <c r="L17" t="n">
-        <v>23.7</v>
-      </c>
-      <c r="M17" t="s">
-        <v>31</v>
-      </c>
+      <c r="L17" t="s">
+        <v>117</v>
+      </c>
+      <c r="M17"/>
       <c r="N17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="B18" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="E18" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="F18" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
@@ -1784,36 +1815,38 @@
         <v>21</v>
       </c>
       <c r="K18"/>
-      <c r="L18" t="n">
-        <v>37</v>
-      </c>
-      <c r="M18"/>
+      <c r="L18" t="s">
+        <v>123</v>
+      </c>
+      <c r="M18" t="s">
+        <v>23</v>
+      </c>
       <c r="N18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O18"/>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B19" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>126</v>
       </c>
       <c r="D19" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="E19" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="F19" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
@@ -1822,38 +1855,34 @@
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>21</v>
+        <v>130</v>
       </c>
       <c r="K19"/>
-      <c r="L19" t="n">
-        <v>32</v>
-      </c>
-      <c r="M19" t="s">
-        <v>22</v>
-      </c>
+      <c r="L19"/>
+      <c r="M19"/>
       <c r="N19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="B20" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="C20" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="D20" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="E20" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="F20" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="G20" t="n">
         <v>1</v>
@@ -1865,37 +1894,37 @@
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="K20"/>
       <c r="L20"/>
       <c r="M20"/>
       <c r="N20" t="s">
-        <v>23</v>
+        <v>130</v>
       </c>
       <c r="O20"/>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="B21" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C21" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D21" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="E21" t="s">
-        <v>124</v>
+        <v>139</v>
       </c>
       <c r="F21" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="G21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -1904,34 +1933,34 @@
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>119</v>
+        <v>21</v>
       </c>
       <c r="K21"/>
       <c r="L21"/>
       <c r="M21"/>
       <c r="N21" t="s">
-        <v>119</v>
+        <v>24</v>
       </c>
       <c r="O21"/>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="B22" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
       <c r="C22" t="s">
-        <v>127</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="E22" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
       <c r="F22" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
       <c r="G22" t="n">
         <v>0</v>
@@ -1946,35 +1975,37 @@
         <v>21</v>
       </c>
       <c r="K22" t="n">
-        <v>0.0001</v>
-      </c>
-      <c r="L22"/>
-      <c r="M22"/>
+        <v>0.00008065</v>
+      </c>
+      <c r="L22" t="s">
+        <v>146</v>
+      </c>
+      <c r="M22" t="s">
+        <v>23</v>
+      </c>
       <c r="N22" t="s">
-        <v>23</v>
-      </c>
-      <c r="O22" t="s">
-        <v>131</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="O22"/>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="B23" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="C23" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
       <c r="E23" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="F23" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
       <c r="G23" t="n">
         <v>0</v>
@@ -1988,32 +2019,38 @@
       <c r="J23" t="s">
         <v>21</v>
       </c>
-      <c r="K23"/>
-      <c r="L23"/>
-      <c r="M23"/>
+      <c r="K23" t="n">
+        <v>0.00002699</v>
+      </c>
+      <c r="L23" t="s">
+        <v>152</v>
+      </c>
+      <c r="M23" t="s">
+        <v>33</v>
+      </c>
       <c r="N23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O23"/>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="B24" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="E24" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="F24" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="G24" t="n">
         <v>0</v>
@@ -2028,37 +2065,37 @@
         <v>21</v>
       </c>
       <c r="K24" t="n">
-        <v>0.00008065</v>
-      </c>
-      <c r="L24" t="n">
-        <v>3.41</v>
+        <v>0.0008</v>
+      </c>
+      <c r="L24" t="s">
+        <v>158</v>
       </c>
       <c r="M24" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="N24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O24"/>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
       <c r="B25" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
       <c r="E25" t="s">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="F25" t="s">
-        <v>146</v>
+        <v>163</v>
       </c>
       <c r="G25" t="n">
         <v>0</v>
@@ -2073,37 +2110,37 @@
         <v>21</v>
       </c>
       <c r="K25" t="n">
-        <v>0.00002699</v>
-      </c>
-      <c r="L25" t="n">
-        <v>13.2</v>
+        <v>0.0009</v>
+      </c>
+      <c r="L25" t="s">
+        <v>164</v>
       </c>
       <c r="M25" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O25"/>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="B26" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="C26" t="s">
         <v>17</v>
       </c>
       <c r="D26" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="E26" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="F26" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="G26" t="n">
         <v>0</v>
@@ -2118,37 +2155,37 @@
         <v>21</v>
       </c>
       <c r="K26" t="n">
-        <v>0.0009</v>
-      </c>
-      <c r="L26" t="n">
-        <v>27.2</v>
+        <v>0</v>
+      </c>
+      <c r="L26" t="s">
+        <v>170</v>
       </c>
       <c r="M26" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="N26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O26"/>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="B27" t="s">
-        <v>153</v>
+        <v>172</v>
       </c>
       <c r="C27" t="s">
         <v>17</v>
       </c>
       <c r="D27" t="s">
-        <v>154</v>
+        <v>173</v>
       </c>
       <c r="E27" t="s">
-        <v>155</v>
+        <v>174</v>
       </c>
       <c r="F27" t="s">
-        <v>156</v>
+        <v>175</v>
       </c>
       <c r="G27" t="n">
         <v>0</v>
@@ -2163,37 +2200,39 @@
         <v>21</v>
       </c>
       <c r="K27" t="n">
-        <v>0</v>
-      </c>
-      <c r="L27" t="n">
-        <v>23.3</v>
+        <v>0.0002</v>
+      </c>
+      <c r="L27" t="s">
+        <v>22</v>
       </c>
       <c r="M27" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="N27" t="s">
-        <v>23</v>
-      </c>
-      <c r="O27"/>
+        <v>24</v>
+      </c>
+      <c r="O27" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="B28" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="C28" t="s">
         <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="E28" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="F28" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="G28" t="n">
         <v>0</v>
@@ -2208,37 +2247,37 @@
         <v>21</v>
       </c>
       <c r="K28" t="n">
-        <v>0.000009069</v>
-      </c>
-      <c r="L28" t="n">
-        <v>29.3</v>
+        <v>0.00006266</v>
+      </c>
+      <c r="L28" t="s">
+        <v>182</v>
       </c>
       <c r="M28" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N28" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O28"/>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>162</v>
+        <v>183</v>
       </c>
       <c r="B29" t="s">
-        <v>163</v>
+        <v>184</v>
       </c>
       <c r="C29" t="s">
         <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>164</v>
+        <v>185</v>
       </c>
       <c r="E29" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
       <c r="F29" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
       <c r="G29" t="n">
         <v>0</v>
@@ -2252,40 +2291,36 @@
       <c r="J29" t="s">
         <v>21</v>
       </c>
-      <c r="K29" t="n">
-        <v>0.0002</v>
-      </c>
-      <c r="L29" t="n">
-        <v>34</v>
+      <c r="K29"/>
+      <c r="L29" t="s">
+        <v>188</v>
       </c>
       <c r="M29" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="N29" t="s">
-        <v>23</v>
-      </c>
-      <c r="O29" t="s">
-        <v>167</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="O29"/>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>168</v>
+        <v>189</v>
       </c>
       <c r="B30" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
       </c>
       <c r="D30" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="E30" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="F30" t="s">
-        <v>172</v>
+        <v>130</v>
       </c>
       <c r="G30" t="n">
         <v>0</v>
@@ -2299,38 +2334,32 @@
       <c r="J30" t="s">
         <v>21</v>
       </c>
-      <c r="K30" t="n">
-        <v>0.00006266</v>
-      </c>
-      <c r="L30" t="n">
-        <v>6.974</v>
-      </c>
-      <c r="M30" t="s">
-        <v>31</v>
-      </c>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
       <c r="N30" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O30"/>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
       <c r="B31" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
       <c r="C31" t="s">
         <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="E31" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
       <c r="F31" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="G31" t="n">
         <v>0</v>
@@ -2344,36 +2373,38 @@
       <c r="J31" t="s">
         <v>21</v>
       </c>
-      <c r="K31"/>
-      <c r="L31" t="n">
-        <v>12.94</v>
+      <c r="K31" t="n">
+        <v>0.00001796</v>
+      </c>
+      <c r="L31" t="s">
+        <v>198</v>
       </c>
       <c r="M31" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="N31" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>178</v>
+        <v>199</v>
       </c>
       <c r="B32" t="s">
-        <v>179</v>
+        <v>200</v>
       </c>
       <c r="C32" t="s">
         <v>17</v>
       </c>
       <c r="D32" t="s">
-        <v>180</v>
+        <v>201</v>
       </c>
       <c r="E32" t="s">
-        <v>181</v>
+        <v>202</v>
       </c>
       <c r="F32" t="s">
-        <v>182</v>
+        <v>203</v>
       </c>
       <c r="G32" t="n">
         <v>0</v>
@@ -2388,37 +2419,37 @@
         <v>21</v>
       </c>
       <c r="K32" t="n">
-        <v>0.000008957</v>
-      </c>
-      <c r="L32" t="n">
-        <v>23.6</v>
+        <v>0.000008958</v>
+      </c>
+      <c r="L32" t="s">
+        <v>204</v>
       </c>
       <c r="M32" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="N32" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O32"/>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="B33" t="s">
-        <v>184</v>
+        <v>206</v>
       </c>
       <c r="C33" t="s">
         <v>17</v>
       </c>
       <c r="D33" t="s">
-        <v>185</v>
+        <v>207</v>
       </c>
       <c r="E33" t="s">
-        <v>186</v>
+        <v>208</v>
       </c>
       <c r="F33" t="s">
-        <v>187</v>
+        <v>130</v>
       </c>
       <c r="G33" t="n">
         <v>0</v>
@@ -2432,38 +2463,32 @@
       <c r="J33" t="s">
         <v>21</v>
       </c>
-      <c r="K33" t="n">
-        <v>0.00005438</v>
-      </c>
-      <c r="L33" t="n">
-        <v>26</v>
-      </c>
-      <c r="M33" t="s">
-        <v>22</v>
-      </c>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
       <c r="N33" t="s">
-        <v>188</v>
+        <v>24</v>
       </c>
       <c r="O33"/>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="B34" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="C34" t="s">
         <v>17</v>
       </c>
       <c r="D34" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
       <c r="E34" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="F34" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
       <c r="G34" t="n">
         <v>0</v>
@@ -2480,35 +2505,37 @@
       <c r="K34" t="n">
         <v>0.00001796</v>
       </c>
-      <c r="L34" t="n">
-        <v>24.5</v>
+      <c r="L34" t="s">
+        <v>214</v>
       </c>
       <c r="M34" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N34" t="s">
-        <v>23</v>
-      </c>
-      <c r="O34"/>
+        <v>24</v>
+      </c>
+      <c r="O34" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>194</v>
+        <v>216</v>
       </c>
       <c r="B35" t="s">
-        <v>195</v>
+        <v>217</v>
       </c>
       <c r="C35" t="s">
         <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>196</v>
+        <v>218</v>
       </c>
       <c r="E35" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="F35" t="s">
-        <v>198</v>
+        <v>220</v>
       </c>
       <c r="G35" t="n">
         <v>0</v>
@@ -2523,37 +2550,37 @@
         <v>21</v>
       </c>
       <c r="K35" t="n">
-        <v>0.000008958</v>
-      </c>
-      <c r="L35" t="n">
-        <v>14.8</v>
+        <v>0.00003588</v>
+      </c>
+      <c r="L35" t="s">
+        <v>221</v>
       </c>
       <c r="M35" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="N35" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O35"/>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>199</v>
+        <v>222</v>
       </c>
       <c r="B36" t="s">
-        <v>200</v>
+        <v>223</v>
       </c>
       <c r="C36" t="s">
         <v>17</v>
       </c>
       <c r="D36" t="s">
-        <v>201</v>
+        <v>224</v>
       </c>
       <c r="E36" t="s">
-        <v>202</v>
+        <v>225</v>
       </c>
       <c r="F36" t="s">
-        <v>203</v>
+        <v>226</v>
       </c>
       <c r="G36" t="n">
         <v>0</v>
@@ -2568,37 +2595,37 @@
         <v>21</v>
       </c>
       <c r="K36" t="n">
-        <v>0.00009873</v>
-      </c>
-      <c r="L36" t="n">
-        <v>19.05</v>
+        <v>0.00002704</v>
+      </c>
+      <c r="L36" t="s">
+        <v>227</v>
       </c>
       <c r="M36" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N36" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O36"/>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
       <c r="B37" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="C37" t="s">
-        <v>17</v>
+        <v>126</v>
       </c>
       <c r="D37" t="s">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="E37" t="s">
-        <v>207</v>
+        <v>231</v>
       </c>
       <c r="F37" t="s">
-        <v>208</v>
+        <v>232</v>
       </c>
       <c r="G37" t="n">
         <v>0</v>
@@ -2612,111 +2639,13 @@
       <c r="J37" t="s">
         <v>21</v>
       </c>
-      <c r="K37" t="n">
-        <v>0.00001796</v>
-      </c>
-      <c r="L37" t="n">
-        <v>21.9</v>
-      </c>
-      <c r="M37" t="s">
-        <v>31</v>
-      </c>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
       <c r="N37" t="s">
-        <v>23</v>
-      </c>
-      <c r="O37" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s">
-        <v>210</v>
-      </c>
-      <c r="B38" t="s">
-        <v>211</v>
-      </c>
-      <c r="C38" t="s">
-        <v>17</v>
-      </c>
-      <c r="D38" t="s">
-        <v>212</v>
-      </c>
-      <c r="E38" t="s">
-        <v>213</v>
-      </c>
-      <c r="F38" t="s">
-        <v>214</v>
-      </c>
-      <c r="G38" t="n">
-        <v>0</v>
-      </c>
-      <c r="H38" t="n">
-        <v>0</v>
-      </c>
-      <c r="I38" t="n">
-        <v>0</v>
-      </c>
-      <c r="J38" t="s">
-        <v>21</v>
-      </c>
-      <c r="K38" t="n">
-        <v>0.00003588</v>
-      </c>
-      <c r="L38" t="n">
-        <v>23.4</v>
-      </c>
-      <c r="M38" t="s">
-        <v>22</v>
-      </c>
-      <c r="N38" t="s">
-        <v>23</v>
-      </c>
-      <c r="O38"/>
-    </row>
-    <row r="39">
-      <c r="A39" t="s">
-        <v>215</v>
-      </c>
-      <c r="B39" t="s">
-        <v>216</v>
-      </c>
-      <c r="C39" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" t="s">
-        <v>217</v>
-      </c>
-      <c r="E39" t="s">
-        <v>218</v>
-      </c>
-      <c r="F39" t="s">
-        <v>219</v>
-      </c>
-      <c r="G39" t="n">
-        <v>0</v>
-      </c>
-      <c r="H39" t="n">
-        <v>0</v>
-      </c>
-      <c r="I39" t="n">
-        <v>0</v>
-      </c>
-      <c r="J39" t="s">
-        <v>21</v>
-      </c>
-      <c r="K39" t="n">
-        <v>0.00002704</v>
-      </c>
-      <c r="L39" t="n">
-        <v>25.3</v>
-      </c>
-      <c r="M39" t="s">
-        <v>31</v>
-      </c>
-      <c r="N39" t="s">
-        <v>23</v>
-      </c>
-      <c r="O39"/>
+        <v>24</v>
+      </c>
+      <c r="O37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>